<commit_message>
osm api request feature done and fixed coordinates marking error
</commit_message>
<xml_diff>
--- a/gmr_scraper/input/hand_written_urls.xlsx
+++ b/gmr_scraper/input/hand_written_urls.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd83645bc27473e1/桌面/gps/google-maps-reviews-scraper/gmr_scraper/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd83645bc27473e1/桌面/gps/Urban/gmr_scraper/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{CA72C847-60A4-4B66-810C-31E7FC66AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9BFDC34-2473-47E0-9D87-381D12A2DC9A}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{CA72C847-60A4-4B66-810C-31E7FC66AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{531C594E-68F0-4BD5-B5E3-25EB2D2FBAE7}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15300" xr2:uid="{601B72FC-55FB-4AE9-B4A0-A65D316F4FA8}"/>
   </bookViews>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
-    <t>X_Cor</t>
-  </si>
-  <si>
-    <t>Y_Cor</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -102,6 +96,12 @@
   </si>
   <si>
     <t>official</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -167,10 +167,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,114 +469,114 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
general sentiment analysis done, but hard to say if it is useful
</commit_message>
<xml_diff>
--- a/gmr_scraper/input/hand_written_urls.xlsx
+++ b/gmr_scraper/input/hand_written_urls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoyamaxx/Desktop/Repo/Urban/gmr_scraper/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd83645bc27473e1/桌面/gps/Urban/gmr_scraper/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A12A2A-C8D8-F449-88CA-0A51EF163E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{66A12A2A-C8D8-F449-88CA-0A51EF163E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{210B33FF-999E-46D9-9355-6139483122B7}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2680" windowWidth="28800" windowHeight="15300" xr2:uid="{601B72FC-55FB-4AE9-B4A0-A65D316F4FA8}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{601B72FC-55FB-4AE9-B4A0-A65D316F4FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
   <si>
     <t>URL</t>
   </si>
@@ -150,18 +150,90 @@
     <t>https://www.google.com/maps/place/Youthland+Outdoor+Playground/@52.3604931,4.9530092,16.83z/data=!4m8!3m7!1s0x47c609469d4a9e0b:0x9f44837f90349920!8m2!3d52.3586717!4d4.9566106!9m1!1b1!16s%2Fg%2F119w_39n7?entry=ttu</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/Park+de+Oeverlanden/@52.3354292,4.8243266,14.54z/data=!4m8!3m7!1s0x47c5e191a0a3dd53:0x177523d8f899245f!8m2!3d52.3353729!4d4.8234372!9m1!1b1!16s%2Fg%2F1hl3grhns?entry=ttu</t>
+    <t>Nieuwemeer</t>
+  </si>
+  <si>
+    <t>Marineterrein</t>
+  </si>
+  <si>
+    <t>Nieuwe Diep</t>
+  </si>
+  <si>
+    <t>Ouderkerkerplas Strand</t>
+  </si>
+  <si>
+    <t>Ouderkerkerplas</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Ouderkerkerplas+Strand/@52.2920434,4.9246177,16z/data=!4m8!3m7!1s0x47c60b0ea07204f5:0x1d4def15104fa3c8!8m2!3d52.2949966!4d4.9295992!9m1!1b1!16s%2Fg%2F11gzr83s1?entry=ttu</t>
+  </si>
+  <si>
+    <t>unofficial</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Ouderkerkerplas/@52.2934374,4.9268533,16.75z/data=!4m18!1m9!3m8!1s0x47c60b0ea07204f5:0x1d4def15104fa3c8!2sOuderkerkerplas+Strand!8m2!3d52.2949966!4d4.9295992!9m1!1b1!16s%2Fg%2F11gzr83s1!3m7!1s0x47c60b1c059db9ab:0x3bf5d42756758b92!8m2!3d52.2943402!4d4.9346832!9m1!1b1!16s%2Fg%2F11gjmxg0lc?entry=ttu</t>
+  </si>
+  <si>
+    <t>Grote Vijver</t>
+  </si>
+  <si>
+    <t>Play island</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Play+island/@52.3209209,4.8264294,17z/data=!4m18!1m9!3m8!1s0x47c5e1b9311bc919:0x157c700ba3e7c974!2sGrote+Vijver!8m2!3d52.3207148!4d4.8292477!9m1!1b1!16s%2Fg%2F1tmgbmll!3m7!1s0x47c5e1bead6baaa5:0x58b5020d1d28d462!8m2!3d52.3215406!4d4.8276456!9m1!1b1!16s%2Fg%2F11g6bqp9ry?entry=ttu</t>
+  </si>
+  <si>
+    <t>Location_Unique</t>
+  </si>
+  <si>
+    <t>Erasmuspark</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Erasmuspark/@52.3765421,4.8448668,14.5z/data=!4m18!1m9!3m8!1s0x47c5e34df7d1a385:0xdda68f0d250f58a8!2sErasmuspark!8m2!3d52.3746222!4d4.8515531!9m1!1b1!16s%2Fg%2F11gh6b_c8h!3m7!1s0x47c5e34df7d1a385:0xdda68f0d250f58a8!8m2!3d52.3746222!4d4.8515531!9m1!1b1!16s%2Fg%2F11gh6b_c8h?entry=ttu</t>
+  </si>
+  <si>
+    <t>De Ceuvel</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Caf%C3%A9+de+Ceuvel/@52.3922115,4.9037356,16z/data=!4m8!3m7!1s0x47c6084e6daacae3:0x128980ceff49bdd8!8m2!3d52.3933105!4d4.9106865!9m1!1b1!16s%2Fg%2F11bbrks_3s?entry=ttu</t>
+  </si>
+  <si>
+    <t>Park schinkeleilanden</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Park+schinkeleilanden/@52.3444785,4.840123,14.5z/data=!4m8!3m7!1s0x47c5e1642ffa8f13:0x96a0ee3050ca97ab!8m2!3d52.3438773!4d4.8500159!9m1!1b1!16s%2Fg%2F11r0n4v_7l?entry=ttu</t>
+  </si>
+  <si>
+    <t>Beach De Hoge Dijk</t>
+  </si>
+  <si>
+    <t>De Hoge Dijk</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Strand+De+Hoge+Dijk/@52.2862557,4.9610664,16.75z/data=!4m8!3m7!1s0x47c60dc6c9ceb023:0xc0f0f272e79d002a!8m2!3d52.2863726!4d4.966084!9m1!1b1!16s%2Fg%2F11h4jb926b?entry=ttu</t>
+  </si>
+  <si>
+    <t>Park Somerlust</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Park+Somerlust/@52.3409612,4.9152788,18.01z/data=!4m8!3m7!1s0x47c60bebadfa153d:0x595a9367bc47551c!8m2!3d52.3408167!4d4.9175899!9m1!1b1!16s%2Fg%2F11cp5_2hwd?entry=ttu</t>
+  </si>
+  <si>
+    <t>Stadshaven Amstelkwartier</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Stadshaven+Amstelkwartier/@52.34103,4.9158689,18z/data=!4m18!1m9!3m8!1s0x47c60bebadfa153d:0x595a9367bc47551c!2sPark+Somerlust!8m2!3d52.3408167!4d4.9175899!9m1!1b1!16s%2Fg%2F11cp5_2hwd!3m7!1s0x47c60bd4e0729b59:0xe0b81330b3886436!8m2!3d52.3417628!4d4.9184656!9m1!1b1!16s%2Fg%2F11cn32t72m?entry=ttu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -170,16 +242,23 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -204,9 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -522,211 +602,374 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5BF9C9-3C0B-4C56-9A00-22778407D0EA}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
         <v>34</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
         <v>36</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>24</v>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.google.com/maps/place/Gaasperplas/@52.3069241,4.9864444,16z/data=!4m12!1m2!2m1!1sGaasperplas!3m8!1s0x47c60c5dbd560937:0xd8ce181a2c1f975b!8m2!3d52.3058653!4d4.994065!9m1!1b1!15sCgtHYWFzcGVycGxhc1oNIgtnYWFzcGVycGxhc5IBBGxha2WaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUmhYelpwWkVGbkVBReABAA!16s%2Fg%2F11bc656tmn?entry=ttu" xr:uid="{91F9A254-FA60-4000-8EE9-46438ACAB047}"/>
+    <hyperlink ref="E6" r:id="rId1" display="https://www.google.com/maps/place/Park+de+Oeverlanden/@52.3349228,4.8191074,15.5z/data=!4m18!1m9!3m8!1s0x47c5e193882abb27:0x8a43187011b73614!2sHet+Nieuwe+Meer!8m2!3d52.3310779!4d4.8202918!9m1!1b1!16s%2Fg%2F121fqn0b!3m7!1s0x47c5e191a0a3dd53:0x177523d8f899245f!8m2!3d52.3353729!4d4.8234372!9m1!1b1!16s%2Fg%2F1hl3grhns?entry=ttu" xr:uid="{9F1DA66A-3C5B-4556-A174-10F6E1FDCD48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>

</xml_diff>